<commit_message>
To run the whole suite
</commit_message>
<xml_diff>
--- a/executioninfo/input-data/TestSuite.xlsx
+++ b/executioninfo/input-data/TestSuite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>SuiteName</t>
   </si>
@@ -68,9 +68,6 @@
 d. Change Password
 e. Add Email Address
 f. Remove Email Address</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -671,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="105" x14ac:dyDescent="0.2">
@@ -682,7 +679,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="106" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>